<commit_message>
Updated TEI zeros with NaN's
</commit_message>
<xml_diff>
--- a/v1.7_SFN_Covariates.xlsx
+++ b/v1.7_SFN_Covariates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avidachs/Documents/GitHub/rf1-sra-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF536DD0-3404-7F41-AB04-5470E773339B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDE9D9C-0185-9546-8570-F8E4888E549C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E21B9450-44FE-AB4C-A453-866E41E6C653}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{E21B9450-44FE-AB4C-A453-866E41E6C653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="150">
   <si>
     <t>tania_subid</t>
   </si>
@@ -844,10 +844,10 @@
   <dimension ref="A1:EI71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AG25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AR11" sqref="AR11"/>
+      <selection pane="bottomRight" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2162,20 +2162,20 @@
       <c r="P4">
         <v>0</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
+      <c r="Q4" t="s">
+        <v>134</v>
+      </c>
+      <c r="R4" t="s">
+        <v>134</v>
+      </c>
+      <c r="S4" t="s">
+        <v>134</v>
+      </c>
+      <c r="T4" t="s">
+        <v>134</v>
+      </c>
+      <c r="U4" t="s">
+        <v>134</v>
       </c>
       <c r="V4">
         <v>33</v>
@@ -2581,20 +2581,20 @@
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
+      <c r="Q5" t="s">
+        <v>134</v>
+      </c>
+      <c r="R5" t="s">
+        <v>134</v>
+      </c>
+      <c r="S5" t="s">
+        <v>134</v>
+      </c>
+      <c r="T5" t="s">
+        <v>134</v>
+      </c>
+      <c r="U5" t="s">
+        <v>134</v>
       </c>
       <c r="V5">
         <v>10</v>
@@ -3419,20 +3419,20 @@
       <c r="P7">
         <v>0</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
+      <c r="Q7" t="s">
+        <v>134</v>
+      </c>
+      <c r="R7" t="s">
+        <v>134</v>
+      </c>
+      <c r="S7" t="s">
+        <v>134</v>
+      </c>
+      <c r="T7" t="s">
+        <v>134</v>
+      </c>
+      <c r="U7" t="s">
+        <v>134</v>
       </c>
       <c r="V7">
         <v>5</v>
@@ -3838,20 +3838,20 @@
       <c r="P8">
         <v>0</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
+      <c r="Q8" t="s">
+        <v>134</v>
+      </c>
+      <c r="R8" t="s">
+        <v>134</v>
+      </c>
+      <c r="S8" t="s">
+        <v>134</v>
+      </c>
+      <c r="T8" t="s">
+        <v>134</v>
+      </c>
+      <c r="U8" t="s">
+        <v>134</v>
       </c>
       <c r="V8">
         <v>37</v>
@@ -5095,20 +5095,20 @@
       <c r="P11">
         <v>0</v>
       </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
+      <c r="Q11" t="s">
+        <v>134</v>
+      </c>
+      <c r="R11" t="s">
+        <v>134</v>
+      </c>
+      <c r="S11" t="s">
+        <v>134</v>
+      </c>
+      <c r="T11" t="s">
+        <v>134</v>
+      </c>
+      <c r="U11" t="s">
+        <v>134</v>
       </c>
       <c r="V11">
         <v>20</v>
@@ -5933,20 +5933,20 @@
       <c r="P13">
         <v>0</v>
       </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
+      <c r="Q13" t="s">
+        <v>134</v>
+      </c>
+      <c r="R13" t="s">
+        <v>134</v>
+      </c>
+      <c r="S13" t="s">
+        <v>134</v>
+      </c>
+      <c r="T13" t="s">
+        <v>134</v>
+      </c>
+      <c r="U13" t="s">
+        <v>134</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -6771,20 +6771,20 @@
       <c r="P15">
         <v>0</v>
       </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
+      <c r="Q15" t="s">
+        <v>134</v>
+      </c>
+      <c r="R15" t="s">
+        <v>134</v>
+      </c>
+      <c r="S15" t="s">
+        <v>134</v>
+      </c>
+      <c r="T15" t="s">
+        <v>134</v>
+      </c>
+      <c r="U15" t="s">
+        <v>134</v>
       </c>
       <c r="V15">
         <v>18</v>
@@ -13894,20 +13894,20 @@
       <c r="P32">
         <v>0</v>
       </c>
-      <c r="Q32">
-        <v>0</v>
-      </c>
-      <c r="R32">
-        <v>0</v>
-      </c>
-      <c r="S32">
-        <v>0</v>
-      </c>
-      <c r="T32">
-        <v>0</v>
-      </c>
-      <c r="U32">
-        <v>0</v>
+      <c r="Q32" t="s">
+        <v>134</v>
+      </c>
+      <c r="R32" t="s">
+        <v>134</v>
+      </c>
+      <c r="S32" t="s">
+        <v>134</v>
+      </c>
+      <c r="T32" t="s">
+        <v>134</v>
+      </c>
+      <c r="U32" t="s">
+        <v>134</v>
       </c>
       <c r="V32">
         <v>0</v>
@@ -18084,20 +18084,20 @@
       <c r="P42">
         <v>0</v>
       </c>
-      <c r="Q42">
-        <v>0</v>
-      </c>
-      <c r="R42">
-        <v>0</v>
-      </c>
-      <c r="S42">
-        <v>0</v>
-      </c>
-      <c r="T42">
-        <v>0</v>
-      </c>
-      <c r="U42">
-        <v>0</v>
+      <c r="Q42" t="s">
+        <v>134</v>
+      </c>
+      <c r="R42" t="s">
+        <v>134</v>
+      </c>
+      <c r="S42" t="s">
+        <v>134</v>
+      </c>
+      <c r="T42" t="s">
+        <v>134</v>
+      </c>
+      <c r="U42" t="s">
+        <v>134</v>
       </c>
       <c r="V42">
         <v>4</v>
@@ -28978,20 +28978,20 @@
       <c r="P68">
         <v>0</v>
       </c>
-      <c r="Q68">
-        <v>0</v>
-      </c>
-      <c r="R68">
-        <v>0</v>
-      </c>
-      <c r="S68">
-        <v>0</v>
-      </c>
-      <c r="T68">
-        <v>0</v>
-      </c>
-      <c r="U68">
-        <v>0</v>
+      <c r="Q68" t="s">
+        <v>134</v>
+      </c>
+      <c r="R68" t="s">
+        <v>134</v>
+      </c>
+      <c r="S68" t="s">
+        <v>134</v>
+      </c>
+      <c r="T68" t="s">
+        <v>134</v>
+      </c>
+      <c r="U68" t="s">
+        <v>134</v>
       </c>
       <c r="V68">
         <v>0</v>

</xml_diff>

<commit_message>
updated NBS zero to NaN for Jimmy
</commit_message>
<xml_diff>
--- a/v1.7_SFN_Covariates.xlsx
+++ b/v1.7_SFN_Covariates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avidachs/Documents/GitHub/rf1-sra-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDE9D9C-0185-9546-8570-F8E4888E549C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A353158-77EB-874F-8828-3760BC216A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{E21B9450-44FE-AB4C-A453-866E41E6C653}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="150">
   <si>
     <t>tania_subid</t>
   </si>
@@ -844,10 +844,10 @@
   <dimension ref="A1:EI71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Z29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q13" sqref="Q13"/>
+      <selection pane="bottomRight" activeCell="AO49" sqref="AO49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20670,8 +20670,8 @@
       <c r="AN48">
         <v>0</v>
       </c>
-      <c r="AO48">
-        <v>0</v>
+      <c r="AO48" t="s">
+        <v>134</v>
       </c>
       <c r="AP48">
         <v>0</v>

</xml_diff>

<commit_message>
v1.8 updated zero values to NaNs
The data coming from the RF1 project was missing NaNs
</commit_message>
<xml_diff>
--- a/v1.7_SFN_Covariates.xlsx
+++ b/v1.7_SFN_Covariates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avidachs/Documents/GitHub/rf1-sra-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A353158-77EB-874F-8828-3760BC216A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906B4187-3ECD-CB42-92F6-57064E21B8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{E21B9450-44FE-AB4C-A453-866E41E6C653}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{E21B9450-44FE-AB4C-A453-866E41E6C653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,9 +524,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,16 +845,17 @@
   <dimension ref="A1:EI71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Z29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AT2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO49" sqref="AO49"/>
+      <selection pane="bottomRight" activeCell="CL9" sqref="CL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="83" max="83" width="10.83203125" style="1" customWidth="1"/>
     <col min="84" max="84" width="10.83203125" style="1"/>
+    <col min="89" max="90" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:139" x14ac:dyDescent="0.2">
@@ -1121,10 +1123,10 @@
       <c r="CJ1" t="s">
         <v>81</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CK1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="CL1" s="2" t="s">
         <v>83</v>
       </c>
       <c r="CM1" t="s">
@@ -1540,10 +1542,10 @@
       <c r="CJ2">
         <v>47</v>
       </c>
-      <c r="CK2" s="1">
+      <c r="CK2" s="2">
         <v>26</v>
       </c>
-      <c r="CL2" s="1">
+      <c r="CL2" s="2">
         <v>29</v>
       </c>
       <c r="CM2">
@@ -1959,10 +1961,10 @@
       <c r="CJ3">
         <v>41</v>
       </c>
-      <c r="CK3" s="1">
+      <c r="CK3" s="2">
         <v>23</v>
       </c>
-      <c r="CL3" s="1">
+      <c r="CL3" s="2">
         <v>33</v>
       </c>
       <c r="CM3">
@@ -2378,10 +2380,10 @@
       <c r="CJ4">
         <v>53</v>
       </c>
-      <c r="CK4" s="1">
+      <c r="CK4" s="2">
         <v>30</v>
       </c>
-      <c r="CL4" s="1">
+      <c r="CL4" s="2">
         <v>30</v>
       </c>
       <c r="CM4">
@@ -2797,10 +2799,10 @@
       <c r="CJ5">
         <v>41</v>
       </c>
-      <c r="CK5" s="1">
+      <c r="CK5" s="2">
         <v>19</v>
       </c>
-      <c r="CL5" s="1">
+      <c r="CL5" s="2">
         <v>35</v>
       </c>
       <c r="CM5">
@@ -3216,10 +3218,10 @@
       <c r="CJ6">
         <v>33</v>
       </c>
-      <c r="CK6" s="1">
+      <c r="CK6" s="2">
         <v>25</v>
       </c>
-      <c r="CL6" s="1">
+      <c r="CL6" s="2">
         <v>27</v>
       </c>
       <c r="CM6">
@@ -3635,10 +3637,10 @@
       <c r="CJ7">
         <v>0</v>
       </c>
-      <c r="CK7" s="1">
+      <c r="CK7" s="2">
         <v>31</v>
       </c>
-      <c r="CL7" s="1">
+      <c r="CL7" s="2">
         <v>27</v>
       </c>
       <c r="CM7">
@@ -4054,10 +4056,10 @@
       <c r="CJ8">
         <v>62</v>
       </c>
-      <c r="CK8" s="1">
+      <c r="CK8" s="2">
         <v>23</v>
       </c>
-      <c r="CL8" s="1">
+      <c r="CL8" s="2">
         <v>30</v>
       </c>
       <c r="CM8">
@@ -4473,10 +4475,10 @@
       <c r="CJ9">
         <v>39</v>
       </c>
-      <c r="CK9" s="1">
+      <c r="CK9" s="2">
         <v>23</v>
       </c>
-      <c r="CL9" s="1">
+      <c r="CL9" s="2">
         <v>36</v>
       </c>
       <c r="CM9">
@@ -4892,10 +4894,10 @@
       <c r="CJ10">
         <v>45</v>
       </c>
-      <c r="CK10" s="1">
+      <c r="CK10" s="2">
         <v>27</v>
       </c>
-      <c r="CL10" s="1">
+      <c r="CL10" s="2">
         <v>28</v>
       </c>
       <c r="CM10">
@@ -5311,10 +5313,10 @@
       <c r="CJ11">
         <v>36</v>
       </c>
-      <c r="CK11" s="1">
+      <c r="CK11" s="2">
         <v>30</v>
       </c>
-      <c r="CL11" s="1">
+      <c r="CL11" s="2">
         <v>31</v>
       </c>
       <c r="CM11">
@@ -5730,10 +5732,10 @@
       <c r="CJ12">
         <v>47</v>
       </c>
-      <c r="CK12" s="1">
+      <c r="CK12" s="2">
         <v>26</v>
       </c>
-      <c r="CL12" s="1">
+      <c r="CL12" s="2">
         <v>0</v>
       </c>
       <c r="CM12">
@@ -6149,10 +6151,10 @@
       <c r="CJ13">
         <v>42</v>
       </c>
-      <c r="CK13" s="1">
+      <c r="CK13" s="2">
         <v>19</v>
       </c>
-      <c r="CL13" s="1">
+      <c r="CL13" s="2">
         <v>32</v>
       </c>
       <c r="CM13">
@@ -6568,10 +6570,10 @@
       <c r="CJ14">
         <v>42</v>
       </c>
-      <c r="CK14" s="1">
+      <c r="CK14" s="2">
         <v>27</v>
       </c>
-      <c r="CL14" s="1">
+      <c r="CL14" s="2">
         <v>29</v>
       </c>
       <c r="CM14">
@@ -6987,10 +6989,10 @@
       <c r="CJ15">
         <v>43</v>
       </c>
-      <c r="CK15" s="1">
+      <c r="CK15" s="2">
         <v>20</v>
       </c>
-      <c r="CL15" s="1">
+      <c r="CL15" s="2">
         <v>20</v>
       </c>
       <c r="CM15">
@@ -7406,10 +7408,10 @@
       <c r="CJ16">
         <v>44</v>
       </c>
-      <c r="CK16" s="1">
+      <c r="CK16" s="2">
         <v>30</v>
       </c>
-      <c r="CL16" s="1">
+      <c r="CL16" s="2">
         <v>38</v>
       </c>
       <c r="CM16">
@@ -7825,10 +7827,10 @@
       <c r="CJ17">
         <v>36</v>
       </c>
-      <c r="CK17" s="1">
+      <c r="CK17" s="2">
         <v>32</v>
       </c>
-      <c r="CL17" s="1">
+      <c r="CL17" s="2">
         <v>29</v>
       </c>
       <c r="CM17">
@@ -8244,10 +8246,10 @@
       <c r="CJ18">
         <v>56</v>
       </c>
-      <c r="CK18" s="1">
+      <c r="CK18" s="2">
         <v>23</v>
       </c>
-      <c r="CL18" s="1">
+      <c r="CL18" s="2">
         <v>34</v>
       </c>
       <c r="CM18">
@@ -8663,10 +8665,10 @@
       <c r="CJ19">
         <v>54</v>
       </c>
-      <c r="CK19" s="1">
+      <c r="CK19" s="2">
         <v>31</v>
       </c>
-      <c r="CL19" s="1">
+      <c r="CL19" s="2">
         <v>33</v>
       </c>
       <c r="CM19">
@@ -9082,10 +9084,10 @@
       <c r="CJ20">
         <v>52</v>
       </c>
-      <c r="CK20" s="1">
+      <c r="CK20" s="2">
         <v>24</v>
       </c>
-      <c r="CL20" s="1">
+      <c r="CL20" s="2">
         <v>37</v>
       </c>
       <c r="CM20">
@@ -9501,10 +9503,10 @@
       <c r="CJ21">
         <v>42</v>
       </c>
-      <c r="CK21" s="1">
+      <c r="CK21" s="2">
         <v>27</v>
       </c>
-      <c r="CL21" s="1">
+      <c r="CL21" s="2">
         <v>32</v>
       </c>
       <c r="CM21">
@@ -9920,10 +9922,10 @@
       <c r="CJ22">
         <v>55</v>
       </c>
-      <c r="CK22" s="1">
+      <c r="CK22" s="2">
         <v>21</v>
       </c>
-      <c r="CL22" s="1">
+      <c r="CL22" s="2">
         <v>38</v>
       </c>
       <c r="CM22">
@@ -10339,10 +10341,10 @@
       <c r="CJ23">
         <v>31</v>
       </c>
-      <c r="CK23" s="1">
+      <c r="CK23" s="2">
         <v>26</v>
       </c>
-      <c r="CL23" s="1">
+      <c r="CL23" s="2">
         <v>33</v>
       </c>
       <c r="CM23">
@@ -10758,10 +10760,10 @@
       <c r="CJ24">
         <v>42</v>
       </c>
-      <c r="CK24" s="1">
+      <c r="CK24" s="2">
         <v>32</v>
       </c>
-      <c r="CL24" s="1">
+      <c r="CL24" s="2">
         <v>28</v>
       </c>
       <c r="CM24">
@@ -11177,10 +11179,10 @@
       <c r="CJ25">
         <v>48</v>
       </c>
-      <c r="CK25" s="1">
+      <c r="CK25" s="2">
         <v>26</v>
       </c>
-      <c r="CL25" s="1">
+      <c r="CL25" s="2">
         <v>34</v>
       </c>
       <c r="CM25">
@@ -11596,10 +11598,10 @@
       <c r="CJ26">
         <v>29</v>
       </c>
-      <c r="CK26" s="1">
+      <c r="CK26" s="2">
         <v>26</v>
       </c>
-      <c r="CL26" s="1">
+      <c r="CL26" s="2">
         <v>31</v>
       </c>
       <c r="CM26">
@@ -12015,10 +12017,10 @@
       <c r="CJ27">
         <v>35</v>
       </c>
-      <c r="CK27" s="1">
+      <c r="CK27" s="2">
         <v>25</v>
       </c>
-      <c r="CL27" s="1">
+      <c r="CL27" s="2">
         <v>32</v>
       </c>
       <c r="CM27">
@@ -12434,10 +12436,10 @@
       <c r="CJ28">
         <v>58</v>
       </c>
-      <c r="CK28" s="1">
+      <c r="CK28" s="2">
         <v>26</v>
       </c>
-      <c r="CL28" s="1">
+      <c r="CL28" s="2">
         <v>35</v>
       </c>
       <c r="CM28">
@@ -12853,10 +12855,10 @@
       <c r="CJ29">
         <v>59</v>
       </c>
-      <c r="CK29" s="1">
+      <c r="CK29" s="2">
         <v>23</v>
       </c>
-      <c r="CL29" s="1">
+      <c r="CL29" s="2">
         <v>28</v>
       </c>
       <c r="CM29">
@@ -13272,10 +13274,10 @@
       <c r="CJ30">
         <v>52</v>
       </c>
-      <c r="CK30" s="1">
+      <c r="CK30" s="2">
         <v>29</v>
       </c>
-      <c r="CL30" s="1">
+      <c r="CL30" s="2">
         <v>31</v>
       </c>
       <c r="CM30">
@@ -13691,10 +13693,10 @@
       <c r="CJ31">
         <v>47</v>
       </c>
-      <c r="CK31" s="1">
+      <c r="CK31" s="2">
         <v>24</v>
       </c>
-      <c r="CL31" s="1">
+      <c r="CL31" s="2">
         <v>37</v>
       </c>
       <c r="CM31">
@@ -14110,10 +14112,10 @@
       <c r="CJ32">
         <v>29</v>
       </c>
-      <c r="CK32" s="1">
+      <c r="CK32" s="2">
         <v>27</v>
       </c>
-      <c r="CL32" s="1">
+      <c r="CL32" s="2">
         <v>31</v>
       </c>
       <c r="CM32">
@@ -14529,10 +14531,10 @@
       <c r="CJ33">
         <v>38</v>
       </c>
-      <c r="CK33" s="1">
+      <c r="CK33" s="2">
         <v>25</v>
       </c>
-      <c r="CL33" s="1">
+      <c r="CL33" s="2">
         <v>27</v>
       </c>
       <c r="CM33">
@@ -14948,10 +14950,10 @@
       <c r="CJ34">
         <v>41</v>
       </c>
-      <c r="CK34" s="1">
+      <c r="CK34" s="2">
         <v>21</v>
       </c>
-      <c r="CL34" s="1">
+      <c r="CL34" s="2">
         <v>32</v>
       </c>
       <c r="CM34">
@@ -15367,10 +15369,10 @@
       <c r="CJ35">
         <v>31</v>
       </c>
-      <c r="CK35" s="1">
+      <c r="CK35" s="2">
         <v>26</v>
       </c>
-      <c r="CL35" s="1">
+      <c r="CL35" s="2">
         <v>32</v>
       </c>
       <c r="CM35">
@@ -15786,10 +15788,10 @@
       <c r="CJ36">
         <v>31</v>
       </c>
-      <c r="CK36" s="1">
+      <c r="CK36" s="2">
         <v>23</v>
       </c>
-      <c r="CL36" s="1">
+      <c r="CL36" s="2">
         <v>31</v>
       </c>
       <c r="CM36">
@@ -16205,10 +16207,10 @@
       <c r="CJ37">
         <v>45</v>
       </c>
-      <c r="CK37" s="1">
+      <c r="CK37" s="2">
         <v>31</v>
       </c>
-      <c r="CL37" s="1">
+      <c r="CL37" s="2">
         <v>30</v>
       </c>
       <c r="CM37">
@@ -16624,10 +16626,10 @@
       <c r="CJ38">
         <v>34</v>
       </c>
-      <c r="CK38" s="1">
+      <c r="CK38" s="2">
         <v>21</v>
       </c>
-      <c r="CL38" s="1">
+      <c r="CL38" s="2">
         <v>32</v>
       </c>
       <c r="CM38">
@@ -17043,10 +17045,10 @@
       <c r="CJ39">
         <v>0</v>
       </c>
-      <c r="CK39" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL39" s="1">
+      <c r="CK39" s="2">
+        <v>0</v>
+      </c>
+      <c r="CL39" s="2">
         <v>30</v>
       </c>
       <c r="CM39">
@@ -17462,10 +17464,10 @@
       <c r="CJ40">
         <v>43</v>
       </c>
-      <c r="CK40" s="1">
+      <c r="CK40" s="2">
         <v>29</v>
       </c>
-      <c r="CL40" s="1">
+      <c r="CL40" s="2">
         <v>23</v>
       </c>
       <c r="CM40">
@@ -17881,10 +17883,10 @@
       <c r="CJ41">
         <v>41</v>
       </c>
-      <c r="CK41" s="1">
+      <c r="CK41" s="2">
         <v>20</v>
       </c>
-      <c r="CL41" s="1">
+      <c r="CL41" s="2">
         <v>32</v>
       </c>
       <c r="CM41">
@@ -18300,10 +18302,10 @@
       <c r="CJ42">
         <v>38</v>
       </c>
-      <c r="CK42" s="1">
+      <c r="CK42" s="2">
         <v>29</v>
       </c>
-      <c r="CL42" s="1">
+      <c r="CL42" s="2">
         <v>27</v>
       </c>
       <c r="CM42">
@@ -18719,10 +18721,10 @@
       <c r="CJ43">
         <v>46</v>
       </c>
-      <c r="CK43" s="1">
+      <c r="CK43" s="2">
         <v>28</v>
       </c>
-      <c r="CL43" s="1">
+      <c r="CL43" s="2">
         <v>35</v>
       </c>
       <c r="CM43">
@@ -19138,10 +19140,10 @@
       <c r="CJ44">
         <v>53</v>
       </c>
-      <c r="CK44" s="1">
+      <c r="CK44" s="2">
         <v>33</v>
       </c>
-      <c r="CL44" s="1">
+      <c r="CL44" s="2">
         <v>32</v>
       </c>
       <c r="CM44">
@@ -19557,10 +19559,10 @@
       <c r="CJ45">
         <v>40</v>
       </c>
-      <c r="CK45" s="1">
+      <c r="CK45" s="2">
         <v>20</v>
       </c>
-      <c r="CL45" s="1">
+      <c r="CL45" s="2">
         <v>29</v>
       </c>
       <c r="CM45">
@@ -19976,10 +19978,10 @@
       <c r="CJ46">
         <v>60</v>
       </c>
-      <c r="CK46" s="1">
+      <c r="CK46" s="2">
         <v>25</v>
       </c>
-      <c r="CL46" s="1">
+      <c r="CL46" s="2">
         <v>36</v>
       </c>
       <c r="CM46">
@@ -20395,10 +20397,10 @@
       <c r="CJ47">
         <v>50</v>
       </c>
-      <c r="CK47" s="1">
+      <c r="CK47" s="2">
         <v>23</v>
       </c>
-      <c r="CL47" s="1">
+      <c r="CL47" s="2">
         <v>34</v>
       </c>
       <c r="CM47">
@@ -20814,10 +20816,10 @@
       <c r="CJ48">
         <v>29</v>
       </c>
-      <c r="CK48" s="1">
+      <c r="CK48" s="2">
         <v>27</v>
       </c>
-      <c r="CL48" s="1">
+      <c r="CL48" s="2">
         <v>26</v>
       </c>
       <c r="CM48">
@@ -21233,10 +21235,10 @@
       <c r="CJ49">
         <v>38</v>
       </c>
-      <c r="CK49" s="1">
+      <c r="CK49" s="2">
         <v>28</v>
       </c>
-      <c r="CL49" s="1">
+      <c r="CL49" s="2">
         <v>27</v>
       </c>
       <c r="CM49">
@@ -21652,10 +21654,10 @@
       <c r="CJ50">
         <v>59</v>
       </c>
-      <c r="CK50" s="1">
+      <c r="CK50" s="2">
         <v>25</v>
       </c>
-      <c r="CL50" s="1">
+      <c r="CL50" s="2">
         <v>22</v>
       </c>
       <c r="CM50">
@@ -22071,10 +22073,10 @@
       <c r="CJ51">
         <v>0</v>
       </c>
-      <c r="CK51" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL51" s="1">
+      <c r="CK51" s="2">
+        <v>0</v>
+      </c>
+      <c r="CL51" s="2">
         <v>37</v>
       </c>
       <c r="CM51">
@@ -22490,10 +22492,10 @@
       <c r="CJ52">
         <v>59</v>
       </c>
-      <c r="CK52" s="1">
+      <c r="CK52" s="2">
         <v>27</v>
       </c>
-      <c r="CL52" s="1">
+      <c r="CL52" s="2">
         <v>0</v>
       </c>
       <c r="CM52">
@@ -22909,10 +22911,10 @@
       <c r="CJ53">
         <v>0</v>
       </c>
-      <c r="CK53" s="1">
+      <c r="CK53" s="2">
         <v>29</v>
       </c>
-      <c r="CL53" s="1">
+      <c r="CL53" s="2">
         <v>30</v>
       </c>
       <c r="CM53">
@@ -23328,10 +23330,10 @@
       <c r="CJ54">
         <v>45</v>
       </c>
-      <c r="CK54" s="1">
+      <c r="CK54" s="2">
         <v>27</v>
       </c>
-      <c r="CL54" s="1">
+      <c r="CL54" s="2">
         <v>34</v>
       </c>
       <c r="CM54">
@@ -23747,10 +23749,10 @@
       <c r="CJ55">
         <v>57</v>
       </c>
-      <c r="CK55" s="1">
+      <c r="CK55" s="2">
         <v>24</v>
       </c>
-      <c r="CL55" s="1">
+      <c r="CL55" s="2">
         <v>36</v>
       </c>
       <c r="CM55">
@@ -24166,10 +24168,10 @@
       <c r="CJ56">
         <v>42</v>
       </c>
-      <c r="CK56" s="1">
+      <c r="CK56" s="2">
         <v>17</v>
       </c>
-      <c r="CL56" s="1">
+      <c r="CL56" s="2">
         <v>25</v>
       </c>
       <c r="CM56">
@@ -24585,10 +24587,10 @@
       <c r="CJ57">
         <v>51</v>
       </c>
-      <c r="CK57" s="1">
+      <c r="CK57" s="2">
         <v>21</v>
       </c>
-      <c r="CL57" s="1">
+      <c r="CL57" s="2">
         <v>29</v>
       </c>
       <c r="CM57">
@@ -25004,10 +25006,10 @@
       <c r="CJ58">
         <v>57</v>
       </c>
-      <c r="CK58" s="1">
+      <c r="CK58" s="2">
         <v>30</v>
       </c>
-      <c r="CL58" s="1">
+      <c r="CL58" s="2">
         <v>36</v>
       </c>
       <c r="CM58">
@@ -25423,10 +25425,10 @@
       <c r="CJ59">
         <v>54</v>
       </c>
-      <c r="CK59" s="1">
+      <c r="CK59" s="2">
         <v>28</v>
       </c>
-      <c r="CL59" s="1">
+      <c r="CL59" s="2">
         <v>38</v>
       </c>
       <c r="CM59">
@@ -25842,10 +25844,10 @@
       <c r="CJ60">
         <v>50</v>
       </c>
-      <c r="CK60" s="1">
+      <c r="CK60" s="2">
         <v>24</v>
       </c>
-      <c r="CL60" s="1">
+      <c r="CL60" s="2">
         <v>30</v>
       </c>
       <c r="CM60">
@@ -26261,10 +26263,10 @@
       <c r="CJ61">
         <v>55</v>
       </c>
-      <c r="CK61" s="1">
+      <c r="CK61" s="2">
         <v>30</v>
       </c>
-      <c r="CL61" s="1">
+      <c r="CL61" s="2">
         <v>29</v>
       </c>
       <c r="CM61">
@@ -26680,10 +26682,10 @@
       <c r="CJ62">
         <v>38</v>
       </c>
-      <c r="CK62" s="1">
+      <c r="CK62" s="2">
         <v>18</v>
       </c>
-      <c r="CL62" s="1">
+      <c r="CL62" s="2">
         <v>30</v>
       </c>
       <c r="CM62">
@@ -27099,10 +27101,10 @@
       <c r="CJ63">
         <v>38</v>
       </c>
-      <c r="CK63" s="1">
+      <c r="CK63" s="2">
         <v>23</v>
       </c>
-      <c r="CL63" s="1">
+      <c r="CL63" s="2">
         <v>34</v>
       </c>
       <c r="CM63">
@@ -27518,10 +27520,10 @@
       <c r="CJ64">
         <v>49</v>
       </c>
-      <c r="CK64" s="1">
+      <c r="CK64" s="2">
         <v>19</v>
       </c>
-      <c r="CL64" s="1">
+      <c r="CL64" s="2">
         <v>36</v>
       </c>
       <c r="CM64">
@@ -27937,10 +27939,10 @@
       <c r="CJ65">
         <v>43</v>
       </c>
-      <c r="CK65" s="1">
+      <c r="CK65" s="2">
         <v>26</v>
       </c>
-      <c r="CL65" s="1">
+      <c r="CL65" s="2">
         <v>34</v>
       </c>
       <c r="CM65">
@@ -28356,10 +28358,10 @@
       <c r="CJ66">
         <v>29</v>
       </c>
-      <c r="CK66" s="1">
+      <c r="CK66" s="2">
         <v>12</v>
       </c>
-      <c r="CL66" s="1">
+      <c r="CL66" s="2">
         <v>35</v>
       </c>
       <c r="CM66">
@@ -28775,10 +28777,10 @@
       <c r="CJ67">
         <v>54</v>
       </c>
-      <c r="CK67" s="1">
+      <c r="CK67" s="2">
         <v>32</v>
       </c>
-      <c r="CL67" s="1">
+      <c r="CL67" s="2">
         <v>33</v>
       </c>
       <c r="CM67">
@@ -29194,10 +29196,10 @@
       <c r="CJ68">
         <v>50</v>
       </c>
-      <c r="CK68" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL68" s="1">
+      <c r="CK68" s="2">
+        <v>0</v>
+      </c>
+      <c r="CL68" s="2">
         <v>31</v>
       </c>
       <c r="CM68">
@@ -29613,10 +29615,10 @@
       <c r="CJ69">
         <v>24</v>
       </c>
-      <c r="CK69" s="1">
+      <c r="CK69" s="2">
         <v>21</v>
       </c>
-      <c r="CL69" s="1">
+      <c r="CL69" s="2">
         <v>18</v>
       </c>
       <c r="CM69">
@@ -30032,10 +30034,10 @@
       <c r="CJ70">
         <v>44</v>
       </c>
-      <c r="CK70" s="1">
+      <c r="CK70" s="2">
         <v>26</v>
       </c>
-      <c r="CL70" s="1">
+      <c r="CL70" s="2">
         <v>18</v>
       </c>
       <c r="CM70">
@@ -30451,10 +30453,10 @@
       <c r="CJ71">
         <v>32</v>
       </c>
-      <c r="CK71" s="1">
+      <c r="CK71" s="2">
         <v>20</v>
       </c>
-      <c r="CL71" s="1">
+      <c r="CL71" s="2">
         <v>26</v>
       </c>
       <c r="CM71">

</xml_diff>